<commit_message>
code in absolute and moved old code
</commit_message>
<xml_diff>
--- a/Data/history_sums.xlsx
+++ b/Data/history_sums.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,582 +439,538 @@
           <t>GICS Sector Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2008</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2009</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>2010</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>2011</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>2013</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>2014</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>2015</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>2016</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2017</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>2018</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>2020</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>2021</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>2022</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>2023</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Communication Services (n=28)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>581944064</v>
+      </c>
+      <c r="C2" t="n">
+        <v>590175814.58</v>
+      </c>
+      <c r="D2" t="n">
+        <v>592059460.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>664555976</v>
+      </c>
+      <c r="F2" t="n">
+        <v>658782100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>679599415</v>
+      </c>
       <c r="H2" t="n">
-        <v>3600783</v>
+        <v>677562313</v>
       </c>
       <c r="I2" t="n">
-        <v>9907956.189999999</v>
+        <v>665429129</v>
       </c>
       <c r="J2" t="n">
-        <v>10412802.71</v>
+        <v>588855945</v>
       </c>
       <c r="K2" t="n">
-        <v>13118412.67</v>
+        <v>608233927</v>
       </c>
       <c r="L2" t="n">
-        <v>13705179.171</v>
+        <v>532924568</v>
       </c>
       <c r="M2" t="n">
-        <v>23267526.363</v>
-      </c>
-      <c r="N2" t="n">
-        <v>13326328.191</v>
-      </c>
-      <c r="O2" t="n">
-        <v>13812645.77</v>
-      </c>
-      <c r="P2" t="n">
-        <v>13255064.841</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>12200336.278</v>
-      </c>
-      <c r="R2" t="n">
-        <v>2648121</v>
+        <v>515882651</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Consumer Discretionary (n=63)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+          <t>Energy</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>298313668</v>
+      </c>
+      <c r="C3" t="n">
+        <v>287926580</v>
+      </c>
+      <c r="D3" t="n">
+        <v>299205635</v>
+      </c>
+      <c r="E3" t="n">
+        <v>298595077</v>
+      </c>
       <c r="F3" t="n">
-        <v>27191</v>
+        <v>299965059</v>
       </c>
       <c r="G3" t="n">
-        <v>27831</v>
+        <v>294868257</v>
       </c>
       <c r="H3" t="n">
-        <v>7089418.92</v>
+        <v>292524559.9</v>
       </c>
       <c r="I3" t="n">
-        <v>33410978.9</v>
+        <v>316638391.6</v>
       </c>
       <c r="J3" t="n">
-        <v>34293885</v>
+        <v>283417659.4</v>
       </c>
       <c r="K3" t="n">
-        <v>38949287</v>
+        <v>263376165.1</v>
       </c>
       <c r="L3" t="n">
-        <v>37143463.746</v>
+        <v>249759998.4</v>
       </c>
       <c r="M3" t="n">
-        <v>41268955.48</v>
-      </c>
-      <c r="N3" t="n">
-        <v>38098188.459</v>
-      </c>
-      <c r="O3" t="n">
-        <v>33202532.507</v>
-      </c>
-      <c r="P3" t="n">
-        <v>31326253.662</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>34008512.299</v>
-      </c>
-      <c r="R3" t="n">
-        <v>7487515.592999999</v>
+        <v>243581873.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Consumer Staples (n=46)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>838139157.39</v>
+      </c>
+      <c r="C4" t="n">
+        <v>620606862.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>599878911.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>581545599</v>
+      </c>
+      <c r="F4" t="n">
+        <v>597712635</v>
+      </c>
+      <c r="G4" t="n">
+        <v>554976528.2</v>
+      </c>
       <c r="H4" t="n">
-        <v>16128467.99</v>
+        <v>479834096.7</v>
       </c>
       <c r="I4" t="n">
-        <v>32532436</v>
+        <v>373998629.22</v>
       </c>
       <c r="J4" t="n">
-        <v>35347785.491</v>
+        <v>327539963.78</v>
       </c>
       <c r="K4" t="n">
-        <v>39186019.609</v>
+        <v>317210734.18</v>
       </c>
       <c r="L4" t="n">
-        <v>48384675.76</v>
+        <v>306923963.59</v>
       </c>
       <c r="M4" t="n">
-        <v>47508552.457</v>
-      </c>
-      <c r="N4" t="n">
-        <v>44183584.216</v>
-      </c>
-      <c r="O4" t="n">
-        <v>41763272.41</v>
-      </c>
-      <c r="P4" t="n">
-        <v>39363406.888</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>37621439.027</v>
-      </c>
-      <c r="R4" t="n">
-        <v>7913385.32</v>
+        <v>226746392.9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Energy (n=21)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+          <t>Industrials</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>105275251.59</v>
+      </c>
+      <c r="C5" t="n">
+        <v>109905694.95</v>
+      </c>
+      <c r="D5" t="n">
+        <v>102428088.39</v>
+      </c>
+      <c r="E5" t="n">
+        <v>104912618.28</v>
+      </c>
+      <c r="F5" t="n">
+        <v>141529224.34</v>
+      </c>
       <c r="G5" t="n">
-        <v>4159424</v>
+        <v>144019849.4</v>
       </c>
       <c r="H5" t="n">
-        <v>89839561</v>
+        <v>153773079.394</v>
       </c>
       <c r="I5" t="n">
-        <v>288466877.4</v>
+        <v>150110536.69</v>
       </c>
       <c r="J5" t="n">
-        <v>289923359.3</v>
+        <v>106345150.02</v>
       </c>
       <c r="K5" t="n">
-        <v>289828148</v>
+        <v>108847999.87</v>
       </c>
       <c r="L5" t="n">
-        <v>230026010</v>
+        <v>142662082.36</v>
       </c>
       <c r="M5" t="n">
-        <v>229096077.31</v>
-      </c>
-      <c r="N5" t="n">
-        <v>253883419.33</v>
-      </c>
-      <c r="O5" t="n">
-        <v>278621416.09</v>
-      </c>
-      <c r="P5" t="n">
-        <v>253604946.4</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>188597662.77</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
+        <v>155298050.343</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Financials (n=125)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>Consumer Discretionary</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>38746865.32</v>
+      </c>
       <c r="C6" t="n">
-        <v>72533</v>
+        <v>39918511.87</v>
       </c>
       <c r="D6" t="n">
-        <v>39593</v>
+        <v>50678948.492</v>
       </c>
       <c r="E6" t="n">
-        <v>63451</v>
+        <v>44412649.052</v>
       </c>
       <c r="F6" t="n">
-        <v>121544</v>
+        <v>43431315.72</v>
       </c>
       <c r="G6" t="n">
-        <v>318506</v>
+        <v>50196439.474</v>
       </c>
       <c r="H6" t="n">
-        <v>3094539.19</v>
+        <v>42454199.803</v>
       </c>
       <c r="I6" t="n">
-        <v>6300298.33</v>
+        <v>43993761.748</v>
       </c>
       <c r="J6" t="n">
-        <v>6200629.4</v>
+        <v>31809396.887</v>
       </c>
       <c r="K6" t="n">
-        <v>5867027.15</v>
+        <v>31823285.495</v>
       </c>
       <c r="L6" t="n">
-        <v>12122380.416</v>
+        <v>43516996.529</v>
       </c>
       <c r="M6" t="n">
-        <v>6140399.21</v>
-      </c>
-      <c r="N6" t="n">
-        <v>6152830.726</v>
-      </c>
-      <c r="O6" t="n">
-        <v>5126432.632</v>
-      </c>
-      <c r="P6" t="n">
-        <v>4228775.157</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>3893206.678</v>
-      </c>
-      <c r="R6" t="n">
-        <v>36501.92</v>
+        <v>43079145.63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Health Care (n=52)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+          <t>Consumer Staples</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>40565811.81</v>
+      </c>
+      <c r="C7" t="n">
+        <v>41825865.18</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38715754.59</v>
+      </c>
+      <c r="E7" t="n">
+        <v>39340382.05</v>
+      </c>
+      <c r="F7" t="n">
+        <v>38881714.9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>43409521</v>
+      </c>
       <c r="H7" t="n">
-        <v>6975709</v>
+        <v>42507279.1</v>
       </c>
       <c r="I7" t="n">
-        <v>16480785</v>
+        <v>41541285.46</v>
       </c>
       <c r="J7" t="n">
-        <v>18069317.2</v>
+        <v>36771136</v>
       </c>
       <c r="K7" t="n">
-        <v>10220535.52</v>
+        <v>38803846.57</v>
       </c>
       <c r="L7" t="n">
-        <v>10145038.76</v>
+        <v>38327802.77</v>
       </c>
       <c r="M7" t="n">
-        <v>9533716.460000001</v>
-      </c>
-      <c r="N7" t="n">
-        <v>12187840.744</v>
-      </c>
-      <c r="O7" t="n">
-        <v>12474050.499</v>
-      </c>
-      <c r="P7" t="n">
-        <v>11604136.748</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>11122402.635</v>
-      </c>
-      <c r="R7" t="n">
-        <v>368148</v>
+        <v>38753541.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Industrials (n=129)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+          <t>Health Care</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>17418038.3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>13139257</v>
+      </c>
       <c r="D8" t="n">
-        <v>869294</v>
+        <v>11635190</v>
       </c>
       <c r="E8" t="n">
-        <v>917491</v>
+        <v>12906158</v>
       </c>
       <c r="F8" t="n">
-        <v>1030429</v>
+        <v>12491671</v>
       </c>
       <c r="G8" t="n">
-        <v>1686776</v>
+        <v>13768182.16</v>
       </c>
       <c r="H8" t="n">
-        <v>13380103.95</v>
+        <v>13173613.21</v>
       </c>
       <c r="I8" t="n">
-        <v>116404416</v>
+        <v>14707514.46</v>
       </c>
       <c r="J8" t="n">
-        <v>142105927.56</v>
+        <v>14730525.4</v>
       </c>
       <c r="K8" t="n">
-        <v>147284497.47</v>
+        <v>14286593.85</v>
       </c>
       <c r="L8" t="n">
-        <v>143723862.376</v>
+        <v>14170721.69</v>
       </c>
       <c r="M8" t="n">
-        <v>157700963.527</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2151197260.398</v>
-      </c>
-      <c r="O8" t="n">
-        <v>126463840.826</v>
-      </c>
-      <c r="P8" t="n">
-        <v>131602395.804</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>130501196.439</v>
-      </c>
-      <c r="R8" t="n">
-        <v>18636349</v>
+        <v>13452277.16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Information Technology (n=27)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+          <t>Communication Services</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11800487.6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12484653.821</v>
+      </c>
+      <c r="D9" t="n">
+        <v>11663497.321</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13211443.702</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14406681.811</v>
+      </c>
+      <c r="G9" t="n">
+        <v>11951992.605</v>
+      </c>
       <c r="H9" t="n">
-        <v>156693</v>
+        <v>12037311.805</v>
       </c>
       <c r="I9" t="n">
-        <v>2457115</v>
+        <v>10589099.868</v>
       </c>
       <c r="J9" t="n">
-        <v>2366536.52</v>
+        <v>13970307.161</v>
       </c>
       <c r="K9" t="n">
-        <v>3096632</v>
+        <v>13821704.718</v>
       </c>
       <c r="L9" t="n">
-        <v>2982911.16</v>
+        <v>12187168.828</v>
       </c>
       <c r="M9" t="n">
-        <v>3047698.41</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2918574.474</v>
-      </c>
-      <c r="O9" t="n">
-        <v>2680106.39</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2739144.174</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>2776240.791</v>
-      </c>
-      <c r="R9" t="n">
-        <v>35711.73</v>
+        <v>11629413.755</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Materials (n=48)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+          <t>Financials</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6210728.53</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5761185.181</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5389313.061</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5615378.697</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5728582.2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5349890.965</v>
+      </c>
       <c r="H10" t="n">
-        <v>139086473</v>
+        <v>5581691.29</v>
       </c>
       <c r="I10" t="n">
-        <v>577106717.27</v>
+        <v>5481874.93</v>
       </c>
       <c r="J10" t="n">
-        <v>663928235</v>
+        <v>5363295.34</v>
       </c>
       <c r="K10" t="n">
-        <v>663575614.308</v>
+        <v>5277106.4</v>
       </c>
       <c r="L10" t="n">
-        <v>650329616.01</v>
+        <v>4856678.94</v>
       </c>
       <c r="M10" t="n">
-        <v>625078655.01</v>
-      </c>
-      <c r="N10" t="n">
-        <v>598869985.577</v>
-      </c>
-      <c r="O10" t="n">
-        <v>546977545.1700001</v>
-      </c>
-      <c r="P10" t="n">
-        <v>533404014.738</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>468537824.55</v>
-      </c>
-      <c r="R10" t="n">
-        <v>37265529.69</v>
+        <v>4390204.84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Real Estate (n=29)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+          <t>Information Technology</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2549275</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3289628.07</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2994286</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3023280</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3565740.1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3478319.2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3561615.07</v>
+      </c>
       <c r="I11" t="n">
-        <v>234252</v>
+        <v>3559954.82</v>
       </c>
       <c r="J11" t="n">
-        <v>343475.3</v>
+        <v>3530140.572</v>
       </c>
       <c r="K11" t="n">
-        <v>498767.06</v>
+        <v>3481445.811</v>
       </c>
       <c r="L11" t="n">
-        <v>580048.4299999999</v>
+        <v>4056906.63</v>
       </c>
       <c r="M11" t="n">
-        <v>551513.0800000001</v>
-      </c>
-      <c r="N11" t="n">
-        <v>554404.429</v>
-      </c>
-      <c r="O11" t="n">
-        <v>1345497.73</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1327217.1</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>1481921.75</v>
-      </c>
-      <c r="R11" t="n">
-        <v>48456.8</v>
+        <v>3993808.35512</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Utilities (n=31)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+          <t>Real Estate</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>584026.7</v>
+      </c>
+      <c r="C12" t="n">
+        <v>596949.3100000001</v>
+      </c>
+      <c r="D12" t="n">
+        <v>580264.12</v>
+      </c>
+      <c r="E12" t="n">
+        <v>684078.764</v>
+      </c>
+      <c r="F12" t="n">
+        <v>593191.1800000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>688953.9</v>
+      </c>
       <c r="H12" t="n">
-        <v>215170378.64</v>
+        <v>615659.9</v>
       </c>
       <c r="I12" t="n">
-        <v>708135262</v>
+        <v>643961.29</v>
       </c>
       <c r="J12" t="n">
-        <v>671891023</v>
+        <v>1392559.03</v>
       </c>
       <c r="K12" t="n">
-        <v>598738800.64</v>
+        <v>1672113.9</v>
       </c>
       <c r="L12" t="n">
-        <v>534520677.2</v>
+        <v>1860920.775</v>
       </c>
       <c r="M12" t="n">
-        <v>440804438.32</v>
-      </c>
-      <c r="N12" t="n">
-        <v>348819739.513</v>
-      </c>
-      <c r="O12" t="n">
-        <v>345970613.044</v>
-      </c>
-      <c r="P12" t="n">
-        <v>321488519.527</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>289637549.66</v>
-      </c>
-      <c r="R12" t="n">
-        <v>15061969</v>
+        <v>2074813.973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>